<commit_message>
Improve accuracy of cost tracking and billing information exports
Adds support for revised cost codes and disables headers in CSV exports.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/a96d8506-7f59-4184-9ee9-9523e82dd47c.jpg
</commit_message>
<xml_diff>
--- a/exports/CORRECTED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
+++ b/exports/CORRECTED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
@@ -5620,7 +5620,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H93" t="n">
@@ -5680,7 +5680,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -6086,7 +6086,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H101" t="n">
@@ -6140,7 +6140,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H102" t="n">
@@ -6196,7 +6196,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H103" t="n">
@@ -6252,7 +6252,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H104" t="n">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H105" t="n">
@@ -6364,7 +6364,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H106" t="n">
@@ -6420,7 +6420,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H107" t="n">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H108" t="n">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H109" t="n">
@@ -6642,7 +6642,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H111" t="n">
@@ -6696,7 +6696,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H112" t="n">
@@ -6752,7 +6752,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H113" t="n">
@@ -6918,7 +6918,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H116" t="n">
@@ -6972,7 +6972,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H117" t="n">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H118" t="n">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H119" t="n">
@@ -7312,7 +7312,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H123" t="n">
@@ -7366,7 +7366,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H124" t="n">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H125" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H126" t="n">
@@ -7534,7 +7534,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H127" t="n">

</xml_diff>